<commit_message>
RTEMIS-201: Add religion optional for import and another sheet for format.
</commit_message>
<xml_diff>
--- a/modules/rte_mis_student_tracking/assets/students_import.xlsx
+++ b/modules/rte_mis_student_tracking/assets/students_import.xlsx
@@ -5,10 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Template" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Format" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="50">
   <si>
     <t xml:space="preserve">Student Name</t>
   </si>
@@ -58,6 +59,9 @@
     <t xml:space="preserve">Medium</t>
   </si>
   <si>
+    <t xml:space="preserve">Religion</t>
+  </si>
+  <si>
     <t xml:space="preserve">Student name</t>
   </si>
   <si>
@@ -73,7 +77,7 @@
     <t xml:space="preserve">address</t>
   </si>
   <si>
-    <t xml:space="preserve">11 digits UDISE</t>
+    <t xml:space="preserve">11 digits and numeric UDISE</t>
   </si>
   <si>
     <t xml:space="preserve">1st</t>
@@ -86,15 +90,97 @@
   </si>
   <si>
     <t xml:space="preserve">medium</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Not mandatory</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Class</t>
+  </si>
+  <si>
+    <t xml:space="preserve">girl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nursery</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hindi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hindu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">boy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">obc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KG-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">english</t>
+  </si>
+  <si>
+    <t xml:space="preserve">muslim</t>
+  </si>
+  <si>
+    <t xml:space="preserve">transgender</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KG-2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sikh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">st</t>
+  </si>
+  <si>
+    <t xml:space="preserve">christian</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">others</t>
+  </si>
+  <si>
+    <t xml:space="preserve">oc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3rd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4th</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5th</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6th</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7th</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8th</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="dd/mm/yy"/>
+    <numFmt numFmtId="166" formatCode="dd/mm/yy"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -168,7 +254,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -178,6 +264,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -200,20 +290,21 @@
   </sheetPr>
   <dimension ref="A1:AMJ2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="131" zoomScaleNormal="131" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J17" activeCellId="0" sqref="J17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="131" zoomScaleNormal="131" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="14.32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="16.65"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="21.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="19.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="24.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="12.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="14.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="12.83"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -253,6 +344,9 @@
       <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="AMF1" s="0"/>
       <c r="AMG1" s="0"/>
       <c r="AMH1" s="0"/>
@@ -261,40 +355,43 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B2" s="2" t="n">
         <v>43990</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E2" s="0" t="s">
         <v>4</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="K2" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="L2" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
+      </c>
+      <c r="M2" s="0" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -306,4 +403,162 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:AMJ12"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="131" zoomScaleNormal="131" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F15" activeCellId="0" sqref="F15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="12.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="15.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="16.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="18.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="18.66"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="AMF1" s="0"/>
+      <c r="AMG1" s="0"/>
+      <c r="AMH1" s="0"/>
+      <c r="AMI1" s="0"/>
+      <c r="AMJ1" s="0"/>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C8" s="0" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C9" s="0" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C10" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C11" s="0" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C12" s="0" t="s">
+        <v>49</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
RTEMIS-201: Resolved bugs for students import.
</commit_message>
<xml_diff>
--- a/modules/rte_mis_student_tracking/assets/students_import.xlsx
+++ b/modules/rte_mis_student_tracking/assets/students_import.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Template" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="49">
   <si>
     <t xml:space="preserve">Student Name</t>
   </si>
@@ -59,25 +59,25 @@
     <t xml:space="preserve">Medium</t>
   </si>
   <si>
+    <t xml:space="preserve">Application Number</t>
+  </si>
+  <si>
     <t xml:space="preserve">Religion</t>
   </si>
   <si>
-    <t xml:space="preserve">Student name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gender</t>
-  </si>
-  <si>
-    <t xml:space="preserve">caste</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mobile number</t>
-  </si>
-  <si>
-    <t xml:space="preserve">address</t>
-  </si>
-  <si>
-    <t xml:space="preserve">11 digits and numeric UDISE</t>
+    <t xml:space="preserve">Student 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Girl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Parent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test address</t>
   </si>
   <si>
     <t xml:space="preserve">1st</t>
@@ -86,13 +86,16 @@
     <t xml:space="preserve">2nd</t>
   </si>
   <si>
-    <t xml:space="preserve">2021-2022</t>
-  </si>
-  <si>
-    <t xml:space="preserve">medium</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Not mandatory</t>
+    <t xml:space="preserve">2021-22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hindi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">application number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hindu</t>
   </si>
   <si>
     <t xml:space="preserve">Class</t>
@@ -105,12 +108,6 @@
   </si>
   <si>
     <t xml:space="preserve">Nursery</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hindi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hindu</t>
   </si>
   <si>
     <t xml:space="preserve">boy</t>
@@ -177,10 +174,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="dd/mm/yy"/>
-    <numFmt numFmtId="166" formatCode="dd/mm/yy"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -254,7 +250,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -267,7 +263,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -290,11 +290,11 @@
   </sheetPr>
   <dimension ref="A1:AMJ2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="131" zoomScaleNormal="131" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="131" zoomScaleNormal="131" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M5" activeCellId="0" sqref="M5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.82421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.51"/>
@@ -304,7 +304,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="24.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="12.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="14.21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="12.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="19.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="12.83"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -347,7 +348,9 @@
       <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="AMF1" s="0"/>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="AMG1" s="0"/>
       <c r="AMH1" s="0"/>
       <c r="AMI1" s="0"/>
@@ -355,28 +358,28 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B2" s="2" t="n">
-        <v>43990</v>
+        <v>44355</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
+      </c>
+      <c r="F2" s="0" t="n">
+        <v>9304025409</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="H2" s="0" t="s">
         <v>18</v>
+      </c>
+      <c r="H2" s="0" t="n">
+        <v>22012000104</v>
       </c>
       <c r="I2" s="0" t="s">
         <v>19</v>
@@ -392,6 +395,9 @@
       </c>
       <c r="M2" s="0" t="s">
         <v>23</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -412,11 +418,11 @@
   </sheetPr>
   <dimension ref="A1:AMJ12"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="131" zoomScaleNormal="131" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F15" activeCellId="0" sqref="F15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="131" zoomScaleNormal="131" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F20" activeCellId="0" sqref="F20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.18"/>
@@ -435,13 +441,13 @@
         <v>3</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="AMF1" s="0"/>
       <c r="AMG1" s="0"/>
@@ -451,105 +457,105 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="B2" s="3" t="s">
         <v>26</v>
       </c>
+      <c r="B2" s="4" t="s">
+        <v>27</v>
+      </c>
       <c r="C2" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="C3" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="D3" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="E3" s="0" t="s">
         <v>33</v>
-      </c>
-      <c r="E3" s="0" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="C4" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="E4" s="0" t="s">
         <v>37</v>
-      </c>
-      <c r="E4" s="0" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="0" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C5" s="0" t="s">
         <v>19</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C6" s="0" t="s">
         <v>20</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="C7" s="0" t="s">
         <v>43</v>
-      </c>
-      <c r="C7" s="0" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C8" s="0" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C9" s="0" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C10" s="0" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C11" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C12" s="0" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>